<commit_message>
Changed dataset for load to CAISO and NYISO
</commit_message>
<xml_diff>
--- a/output/hydro_data.xlsx
+++ b/output/hydro_data.xlsx
@@ -557,19 +557,19 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>1000.0</v>
       </c>
       <c r="E2">
-        <v>10000000</v>
+        <v>1.0e7</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -581,10 +581,10 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M2">
         <v>100000</v>
@@ -604,13 +604,13 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D3">
         <v>58.04</v>
       </c>
       <c r="E3">
-        <v>10000000</v>
+        <v>1.0e7</v>
       </c>
       <c r="F3">
         <v>11.7</v>
@@ -631,7 +631,7 @@
         <v>2.39</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M3">
         <v>100000</v>
@@ -651,16 +651,16 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>1000</v>
+        <v>1000.0</v>
       </c>
       <c r="D4">
         <v>61.27</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F4">
-        <v>15</v>
+        <v>15.0</v>
       </c>
       <c r="G4">
         <v>0.068</v>
@@ -675,10 +675,10 @@
         <v>49907</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M4">
         <v>100000</v>
@@ -698,13 +698,13 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D5">
         <v>81.6</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F5">
         <v>18.8</v>
@@ -725,7 +725,7 @@
         <v>47.05</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M5">
         <v>100000</v>
@@ -745,13 +745,13 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D6">
         <v>23.92</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F6">
         <v>9.3</v>
@@ -772,7 +772,7 @@
         <v>84.59</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M6">
         <v>100000</v>
@@ -792,16 +792,16 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>1000</v>
+        <v>1000.0</v>
       </c>
       <c r="D7">
-        <v>75</v>
+        <v>75.0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F7">
-        <v>27</v>
+        <v>27.0</v>
       </c>
       <c r="G7">
         <v>0.1</v>
@@ -816,10 +816,10 @@
         <v>49903</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M7">
         <v>100000</v>
@@ -842,10 +842,10 @@
         <v>349450.0</v>
       </c>
       <c r="D8">
-        <v>105</v>
+        <v>105.0</v>
       </c>
       <c r="E8">
-        <v>30000</v>
+        <v>30000.0</v>
       </c>
       <c r="F8">
         <v>123.98</v>
@@ -866,7 +866,7 @@
         <v>899.52</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M8">
         <v>100000</v>
@@ -886,16 +886,16 @@
         <v>22</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D9">
         <v>82.78</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F9">
-        <v>45</v>
+        <v>45.0</v>
       </c>
       <c r="G9">
         <v>0.151</v>
@@ -913,7 +913,7 @@
         <v>47.64</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M9">
         <v>100000</v>
@@ -936,16 +936,16 @@
         <v>18700.0</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>10.0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H10">
         <v>49906</v>
@@ -960,7 +960,7 @@
         <v>21.64</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M10">
         <v>100000</v>
@@ -980,16 +980,16 @@
         <v>24</v>
       </c>
       <c r="C11">
-        <v>37000</v>
+        <v>37000.0</v>
       </c>
       <c r="D11">
         <v>13.04</v>
       </c>
       <c r="E11">
-        <v>10000</v>
+        <v>10000.0</v>
       </c>
       <c r="F11">
-        <v>20</v>
+        <v>20.0</v>
       </c>
       <c r="G11">
         <v>0.426</v>
@@ -1007,7 +1007,7 @@
         <v>25.96</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M11">
         <v>100000</v>
@@ -1027,16 +1027,16 @@
         <v>25</v>
       </c>
       <c r="C12">
-        <v>65000</v>
+        <v>65000.0</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>8.0</v>
       </c>
       <c r="E12">
-        <v>10000</v>
+        <v>10000.0</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>7.0</v>
       </c>
       <c r="G12">
         <v>0.243</v>
@@ -1054,7 +1054,7 @@
         <v>35.71</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M12">
         <v>100000</v>
@@ -1074,16 +1074,16 @@
         <v>26</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D13">
         <v>2.33</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G13">
         <v>0.119</v>
@@ -1101,7 +1101,7 @@
         <v>46.66</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M13">
         <v>100000</v>
@@ -1121,19 +1121,19 @@
         <v>27</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>15.0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H14">
         <v>49912</v>
@@ -1148,7 +1148,7 @@
         <v>49.35</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M14">
         <v>100000</v>
@@ -1168,19 +1168,19 @@
         <v>28</v>
       </c>
       <c r="C15">
-        <v>6000</v>
+        <v>6000.0</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>13.0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H15">
         <v>49911</v>
@@ -1195,7 +1195,7 @@
         <v>27.3</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M15">
         <v>100000</v>
@@ -1215,13 +1215,13 @@
         <v>29</v>
       </c>
       <c r="C16">
-        <v>4000</v>
+        <v>4000.0</v>
       </c>
       <c r="D16">
         <v>80.21</v>
       </c>
       <c r="E16">
-        <v>15000</v>
+        <v>15000.0</v>
       </c>
       <c r="F16">
         <v>66.7</v>
@@ -1242,7 +1242,7 @@
         <v>413.56</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M16">
         <v>100000</v>
@@ -1262,16 +1262,16 @@
         <v>30</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D17">
         <v>65.36</v>
       </c>
       <c r="E17">
-        <v>15000</v>
+        <v>15000.0</v>
       </c>
       <c r="F17">
-        <v>32</v>
+        <v>32.0</v>
       </c>
       <c r="G17">
         <v>0.136</v>
@@ -1286,10 +1286,10 @@
         <v>49906</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M17">
         <v>100000</v>
@@ -1309,16 +1309,16 @@
         <v>31</v>
       </c>
       <c r="C18">
-        <v>1000</v>
+        <v>1000.0</v>
       </c>
       <c r="D18">
         <v>102.12</v>
       </c>
       <c r="E18">
-        <v>3000</v>
+        <v>3000.0</v>
       </c>
       <c r="F18">
-        <v>25</v>
+        <v>25.0</v>
       </c>
       <c r="G18">
         <v>0.068</v>
@@ -1336,7 +1336,7 @@
         <v>241.79</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M18">
         <v>100000</v>
@@ -1356,13 +1356,13 @@
         <v>32</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D19">
         <v>20.02</v>
       </c>
       <c r="E19">
-        <v>1000</v>
+        <v>1000.0</v>
       </c>
       <c r="F19">
         <v>31.71</v>
@@ -1383,7 +1383,7 @@
         <v>1.89</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M19">
         <v>100000</v>
@@ -1409,7 +1409,7 @@
         <v>58.36</v>
       </c>
       <c r="E20">
-        <v>7000</v>
+        <v>7000.0</v>
       </c>
       <c r="F20">
         <v>175.01</v>
@@ -1430,7 +1430,7 @@
         <v>22.46</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M20">
         <v>100000</v>
@@ -1450,16 +1450,16 @@
         <v>34</v>
       </c>
       <c r="C21">
-        <v>582000</v>
+        <v>582000.0</v>
       </c>
       <c r="D21">
         <v>93.37</v>
       </c>
       <c r="E21">
-        <v>7000</v>
+        <v>7000.0</v>
       </c>
       <c r="F21">
-        <v>40</v>
+        <v>40.0</v>
       </c>
       <c r="G21">
         <v>0.119</v>
@@ -1477,7 +1477,7 @@
         <v>456.89</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M21">
         <v>100000</v>
@@ -1497,16 +1497,16 @@
         <v>35</v>
       </c>
       <c r="C22">
-        <v>187000</v>
+        <v>187000.0</v>
       </c>
       <c r="D22">
         <v>30.06</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F22">
-        <v>25</v>
+        <v>25.0</v>
       </c>
       <c r="G22">
         <v>0.231</v>
@@ -1524,7 +1524,7 @@
         <v>280.5</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M22">
         <v>100000</v>
@@ -1544,13 +1544,13 @@
         <v>36</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D23">
         <v>10.06</v>
       </c>
       <c r="E23">
-        <v>2000</v>
+        <v>2000.0</v>
       </c>
       <c r="F23">
         <v>2.5</v>
@@ -1571,7 +1571,7 @@
         <v>103.5</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M23">
         <v>100000</v>
@@ -1591,19 +1591,19 @@
         <v>37</v>
       </c>
       <c r="C24">
-        <v>52000</v>
+        <v>52000.0</v>
       </c>
       <c r="D24">
-        <v>32</v>
+        <v>32.0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H24">
         <v>49931</v>
@@ -1618,7 +1618,7 @@
         <v>41.62</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M24">
         <v>100000</v>
@@ -1638,19 +1638,19 @@
         <v>38</v>
       </c>
       <c r="C25">
-        <v>50000</v>
+        <v>50000.0</v>
       </c>
       <c r="D25">
-        <v>11</v>
+        <v>11.0</v>
       </c>
       <c r="E25">
-        <v>10000</v>
+        <v>10000.0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H25">
         <v>49928</v>
@@ -1665,7 +1665,7 @@
         <v>172.76</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M25">
         <v>100000</v>
@@ -1685,19 +1685,19 @@
         <v>39</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D26">
-        <v>1000</v>
+        <v>1000.0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H26">
         <v>49923</v>
@@ -1712,7 +1712,7 @@
         <v>169.25</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="M26">
         <v>100000</v>

</xml_diff>

<commit_message>
Added activation costs to optimization cost calculation
</commit_message>
<xml_diff>
--- a/output/hydro_data.xlsx
+++ b/output/hydro_data.xlsx
@@ -637,7 +637,7 @@
         <v>100000</v>
       </c>
       <c r="N3">
-        <v>0.56</v>
+        <v>2.0160000000000005</v>
       </c>
       <c r="O3">
         <v>0.0</v>
@@ -684,7 +684,7 @@
         <v>100000</v>
       </c>
       <c r="N4">
-        <v>1.2400000000000002</v>
+        <v>4.464</v>
       </c>
       <c r="O4">
         <v>500.0</v>
@@ -731,7 +731,7 @@
         <v>100000</v>
       </c>
       <c r="N5">
-        <v>1.8800000000000003</v>
+        <v>6.768000000000001</v>
       </c>
       <c r="O5">
         <v>0.0</v>
@@ -778,7 +778,7 @@
         <v>100000</v>
       </c>
       <c r="N6">
-        <v>2.9600000000000004</v>
+        <v>10.656</v>
       </c>
       <c r="O6">
         <v>0.0</v>
@@ -825,7 +825,7 @@
         <v>100000</v>
       </c>
       <c r="N7">
-        <v>2.8800000000000003</v>
+        <v>10.368</v>
       </c>
       <c r="O7">
         <v>500.0</v>
@@ -872,7 +872,7 @@
         <v>100000</v>
       </c>
       <c r="N8">
-        <v>3.2800000000000002</v>
+        <v>11.808000000000002</v>
       </c>
       <c r="O8">
         <v>174725.0</v>
@@ -919,7 +919,7 @@
         <v>100000</v>
       </c>
       <c r="N9">
-        <v>1.51</v>
+        <v>5.436</v>
       </c>
       <c r="O9">
         <v>0.0</v>
@@ -966,7 +966,7 @@
         <v>100000</v>
       </c>
       <c r="N10">
-        <v>3.2800000000000002</v>
+        <v>11.808000000000002</v>
       </c>
       <c r="O10">
         <v>9350.0</v>
@@ -1013,7 +1013,7 @@
         <v>100000</v>
       </c>
       <c r="N11">
-        <v>7.54</v>
+        <v>27.144000000000002</v>
       </c>
       <c r="O11">
         <v>18500.0</v>
@@ -1060,7 +1060,7 @@
         <v>100000</v>
       </c>
       <c r="N12">
-        <v>9.969999999999999</v>
+        <v>35.892</v>
       </c>
       <c r="O12">
         <v>32500.0</v>
@@ -1107,7 +1107,7 @@
         <v>100000</v>
       </c>
       <c r="N13">
-        <v>11.159999999999998</v>
+        <v>40.176</v>
       </c>
       <c r="O13">
         <v>0.0</v>
@@ -1154,7 +1154,7 @@
         <v>100000</v>
       </c>
       <c r="N14">
-        <v>9.969999999999999</v>
+        <v>35.892</v>
       </c>
       <c r="O14">
         <v>0.0</v>
@@ -1201,7 +1201,7 @@
         <v>100000</v>
       </c>
       <c r="N15">
-        <v>7.54</v>
+        <v>27.144000000000002</v>
       </c>
       <c r="O15">
         <v>3000.0</v>
@@ -1248,7 +1248,7 @@
         <v>100000</v>
       </c>
       <c r="N16">
-        <v>5.59</v>
+        <v>20.124000000000002</v>
       </c>
       <c r="O16">
         <v>2000.0</v>
@@ -1295,7 +1295,7 @@
         <v>100000</v>
       </c>
       <c r="N17">
-        <v>4.640000000000001</v>
+        <v>16.704</v>
       </c>
       <c r="O17">
         <v>0.0</v>
@@ -1342,7 +1342,7 @@
         <v>100000</v>
       </c>
       <c r="N18">
-        <v>6.27</v>
+        <v>22.572000000000003</v>
       </c>
       <c r="O18">
         <v>500.0</v>
@@ -1389,7 +1389,7 @@
         <v>100000</v>
       </c>
       <c r="N19">
-        <v>10.67</v>
+        <v>38.412000000000006</v>
       </c>
       <c r="O19">
         <v>0.0</v>
@@ -1436,7 +1436,7 @@
         <v>100000</v>
       </c>
       <c r="N20">
-        <v>14.6</v>
+        <v>52.56</v>
       </c>
       <c r="O20">
         <v>18650.0</v>
@@ -1483,7 +1483,7 @@
         <v>100000</v>
       </c>
       <c r="N21">
-        <v>15.79</v>
+        <v>56.844</v>
       </c>
       <c r="O21">
         <v>291000.0</v>
@@ -1530,7 +1530,7 @@
         <v>100000</v>
       </c>
       <c r="N22">
-        <v>18.099999999999998</v>
+        <v>65.16</v>
       </c>
       <c r="O22">
         <v>93500.0</v>
@@ -1577,7 +1577,7 @@
         <v>100000</v>
       </c>
       <c r="N23">
-        <v>11.36</v>
+        <v>40.89600000000001</v>
       </c>
       <c r="O23">
         <v>0.0</v>
@@ -1624,7 +1624,7 @@
         <v>100000</v>
       </c>
       <c r="N24">
-        <v>10.67</v>
+        <v>38.412000000000006</v>
       </c>
       <c r="O24">
         <v>26000.0</v>
@@ -1671,7 +1671,7 @@
         <v>100000</v>
       </c>
       <c r="N25">
-        <v>11.36</v>
+        <v>40.89600000000001</v>
       </c>
       <c r="O25">
         <v>25000.0</v>
@@ -1718,7 +1718,7 @@
         <v>100000</v>
       </c>
       <c r="N26">
-        <v>10.67</v>
+        <v>38.412000000000006</v>
       </c>
       <c r="O26">
         <v>0.0</v>

</xml_diff>